<commit_message>
refactor: Make OntologyTerm inherit from NamedThing
- OntologyTerm now extends NamedThing class
- Removed duplicate 'id' attribute definition
- Inherits id (as uriorcurie), title, and description from parent
- Maintains label, definition, and ontology as specific attributes

This follows DRY principles and ensures consistent identity management
across all named entities in the schema.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -550,7 +550,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,ascii,thermo_raw"</formula1>
+      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,ascii,thermo_raw,zip"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data"</formula1>
@@ -1304,33 +1304,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>definition</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ontology</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>definition</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ontology</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: Introduce AttributeGroup base class for complex attributes
Created AttributeGroup as abstract base class for value objects/property groups
that don't have independent identity. Classes now inheriting from AttributeGroup:

- MolecularComposition
- BufferComposition
- StorageConditions
- ExperimentalConditions
- DataCollectionStrategy
- QualityMetrics
- ComputeResources
- TechniqueSpecificPreparation (and its subclasses)
- ImageFeature

This provides a clear distinction between:
- NamedThing: Entities with identity (id, title, description)
- AttributeGroup: Complex attributes without independent identity

Benefits:
- Clear semantic separation of entity types
- Consistent inheritance hierarchy
- Potential for shared validation or behavior
- Better schema organization

All existing datasets validate successfully with this change.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -1278,7 +1278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,6 +1292,11 @@
           <t>terms</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1421,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1445,6 +1450,11 @@
           <t>ligands</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1457,7 +1467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,6 +1491,11 @@
           <t>additives</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1493,7 +1508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1520,6 +1535,11 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>atmosphere</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -1539,7 +1559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1591,6 +1611,11 @@
       <c r="I1" t="inlineStr">
         <is>
           <t>plasma_treatment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1655,6 +1680,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>flash_cooling_method</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1708,6 +1738,11 @@
           <t>temperature_control</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1720,6 +1755,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>temperature</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>humidity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>atmosphere</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>beam_energy</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1731,78 +1822,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>temperature</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>humidity</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>pressure</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>atmosphere</t>
+          <t>collection_mode</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>total_frames</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>frame_rate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>total_dose</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>beam_energy</t>
+          <t>dose_per_frame</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>collection_mode</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>total_frames</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>frame_rate</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>total_dose</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>dose_per_frame</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1861,6 +1906,11 @@
           <t>rg</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1873,7 +1923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1900,6 +1950,11 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>storage_gb</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add instruments list to Dataset and change instrument_id to reference Instrument objects
- Added instruments list to Dataset class for storing instrument definitions at dataset level
- Changed instrument_id range from string to Instrument for proper referencing over inlining
- Made Instrument class non-abstract to support Dataset-level instrument definitions
- Updated all example Dataset objects to include instruments list with basic instrument definitions
- Regenerated all schema artifacts including Python dataclasses, JSON Schema, and documentation

This implements option 1 from the issue: having instruments at Dataset level with referencing.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -11,31 +11,32 @@
     <sheet name="Study" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sample" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="SamplePreparation" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="CryoEMInstrument" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="XRayInstrument" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="SAXSInstrument" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="ExperimentRun" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="WorkflowRun" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="DataFile" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Image" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Image2D" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Image3D" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="FTIRImage" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="FluorescenceImage" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="OpticalImage" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="XRFImage" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="ImageFeature" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="OntologyTerm" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="MolecularComposition" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="BufferComposition" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="StorageConditions" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="CryoEMPreparation" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="XRayPreparation" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="SAXSPreparation" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="ExperimentalConditions" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="DataCollectionStrategy" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="QualityMetrics" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="ComputeResources" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Instrument" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CryoEMInstrument" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="XRayInstrument" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SAXSInstrument" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ExperimentRun" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="WorkflowRun" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="DataFile" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Image" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Image2D" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Image3D" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="FTIRImage" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="FluorescenceImage" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="OpticalImage" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="XRFImage" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="ImageFeature" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="OntologyTerm" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="MolecularComposition" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="BufferComposition" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="StorageConditions" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CryoEMPreparation" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="XRayPreparation" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="SAXSPreparation" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="ExperimentalConditions" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="DataCollectionStrategy" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="QualityMetrics" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="ComputeResources" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,31 +458,132 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>instruments</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>studies</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>workflow_code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>workflow_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>experiment_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>processing_level</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>software_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>software_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processing_parameters</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>compute_resources</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>started_at</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>completed_at</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>output_files</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"motion_correction,ctf_estimation,particle_picking,classification_2d,classification_3d,refinement,model_building,phasing,integration,scaling,saxs_analysis,em_2d_classification,mass_spec_deconvolution"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -560,7 +662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -631,7 +733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -712,7 +814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -798,7 +900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -904,7 +1006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1030,7 +1132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1146,7 +1248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1272,7 +1374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1303,7 +1405,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>samples</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sample_preparations</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>instrument_runs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>workflow_runs</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>data_files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>images</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1354,73 +1522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>samples</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sample_preparations</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>instrument_runs</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>workflow_runs</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>data_files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>images</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1461,7 +1563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1502,7 +1604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1553,7 +1655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1632,7 +1734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1698,7 +1800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1749,7 +1851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1805,7 +1907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1861,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1907,52 +2009,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cpu_hours</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>gpu_hours</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>memory_gb</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>storage_gb</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2067,6 +2123,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cpu_hours</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>gpu_hours</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>memory_gb</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>storage_gb</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2134,6 +2236,72 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>instrument_code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>installation_date</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>current_status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"operational,maintenance,offline,commissioning"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2242,7 +2410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2356,7 +2524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2452,7 +2620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2549,100 +2717,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>workflow_code</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>workflow_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>experiment_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>processing_level</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>software_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>software_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_parameters</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>compute_resources</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>started_at</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>completed_at</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>output_files</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"motion_correction,ctf_estimation,particle_picking,classification_2d,classification_3d,refinement,model_building,phasing,integration,scaling,saxs_analysis,em_2d_classification,mass_spec_deconvolution"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add biological context fields to Sample class
This addresses issue #4 by adding organism, anatomy, and cell_type fields
to the Sample class as OntologyTerm references. These fields enable proper
recording of biological source information including:

- organism: Source species (e.g., NCBITaxon:3702 for Arabidopsis)
- anatomy: Anatomical part/tissue (e.g., UBERON:0008945 for leaf)
- cell_type: Cell type when applicable (e.g., CL:0000057 for fibroblast)

The fields are optional to maintain backwards compatibility with existing
examples. This enhances the schema's utility for biomedical applications
requiring structured biological metadata and ontology integration.

Co-authored-by: Chris Mungall <cmungall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -2025,7 +2025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2081,30 +2081,45 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>organism</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>cell_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>parent_sample_id</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>purity_percentage</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>quality_metrics</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Implement type designators for technique-specific sample preparation details
This resolves the issue where rich technique-specific preparation metadata
could not be attached to SamplePreparation objects.

Key changes:
- Added type designator to preparation_type slot (designates_type: true)
- Made technique-specific classes inherit from SamplePreparation:
  * CryoEMPreparation is_a SamplePreparation
  * XRayPreparation is_a SamplePreparation
  * SAXSPreparation is_a SamplePreparation
- Updated example data to demonstrate new capabilities
- Generated polymorphic JSON schema validation

This enables capturing critical preparation metadata:
- Cryo-EM: blot_time, blot_force, grid_type, vitrification_method, etc.
- X-ray: crystallization_method, crystal_size, cryoprotectant, etc.
- SAXS: concentration_series, buffer_matching_protocol, etc.

Resolves #3

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Chris Mungall <cmungall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -1661,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1716,6 +1716,41 @@
         </is>
       </c>
       <c r="J1" t="inlineStr">
+        <is>
+          <t>preparation_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1740,7 +1775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,6 +1820,41 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>preparation_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1806,7 +1876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1841,6 +1911,41 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
+        <is>
+          <t>preparation_type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2241,11 +2346,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,sans,protein_expression,protein_purification,negative_stain"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Implement type designator using 'type' field for technique-specific sample preparation
- Rename preparation_type field to 'type' with designates_type: true
- Make CryoEMPreparation, XRayPreparation, SAXSPreparation inherit from SamplePreparation
- Update all example data to use new type designator pattern
- Remove PreparationTypeEnum in favor of string-based type designators
- Generate polymorphic JSON schema with anyOf unions for sample_preparations

This enables capturing rich technique-specific metadata (blot_time, crystallization_method, etc.)
while maintaining proper inheritance and type safety.

Resolves #3

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-authored-by: Chris Mungall <cmungall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/biostride.xlsx
+++ b/assets/excel/biostride.xlsx
@@ -1661,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1716,6 +1716,41 @@
         </is>
       </c>
       <c r="J1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1740,7 +1775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,6 +1820,41 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1806,7 +1876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1841,6 +1911,41 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>preparation_date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>operator_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>protocol_description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2201,7 +2306,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>preparation_type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2241,11 +2346,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,sans,protein_expression,protein_purification,negative_stain"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>